<commit_message>
model and high N case py.
</commit_message>
<xml_diff>
--- a/AMP No Nitrogen - NH4 Additions to Quantify N Contamination.xlsx
+++ b/AMP No Nitrogen - NH4 Additions to Quantify N Contamination.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkm/Documents/Talmy_research/Zinser_and_Ben/Project_1_nutrients_prelim_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkm/Documents/Talmy_research/Zinser_and_Ben/Project_1_nutrient_additions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A3F042-E0BA-9A47-894C-BCE91B256DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE2EEA6-FEA3-754C-BBC8-83745B10D79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="1040" windowWidth="23900" windowHeight="14080" xr2:uid="{3787FD8E-FF35-4CFB-9ADE-A1372B15C76F}"/>
+    <workbookView xWindow="3340" yWindow="1040" windowWidth="23900" windowHeight="14080" activeTab="2" xr2:uid="{3787FD8E-FF35-4CFB-9ADE-A1372B15C76F}"/>
   </bookViews>
   <sheets>
     <sheet name="AMP No N Quant NH4 Trial 3" sheetId="1" r:id="rId1"/>
@@ -447,15 +447,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -463,6 +454,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF21520F-4E0E-4730-B161-A7997D96884F}">
   <dimension ref="A1:AK48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:AK16"/>
     </sheetView>
   </sheetViews>
@@ -857,131 +857,131 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="29" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="29" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="29" t="s">
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="29" t="s">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="29" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="31"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="28"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="29" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="29" t="s">
+      <c r="M3" s="28"/>
+      <c r="N3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30" t="s">
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="29" t="s">
+      <c r="S3" s="28"/>
+      <c r="T3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30" t="s">
+      <c r="U3" s="27"/>
+      <c r="V3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30" t="s">
+      <c r="W3" s="27"/>
+      <c r="X3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="29" t="s">
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30" t="s">
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30" t="s">
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="29" t="s">
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30" t="s">
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="30" t="s">
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AK3" s="31"/>
+      <c r="AK3" s="28"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2475,36 +2475,36 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28" t="s">
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="28" t="s">
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="26"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="28" t="s">
+      <c r="O18" s="30"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="R18" s="26"/>
-      <c r="S18" s="27"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="31"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -3769,30 +3769,30 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="26" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="26" t="s">
+      <c r="E34" s="31"/>
+      <c r="F34" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="26" t="s">
+      <c r="G34" s="31"/>
+      <c r="H34" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="27"/>
-      <c r="J34" s="26" t="s">
+      <c r="I34" s="31"/>
+      <c r="J34" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="27"/>
-      <c r="L34" s="26" t="s">
+      <c r="K34" s="31"/>
+      <c r="L34" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="M34" s="27"/>
+      <c r="M34" s="31"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -4778,6 +4778,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z2:AE2"/>
     <mergeCell ref="AF2:AK2"/>
     <mergeCell ref="L3:M3"/>
@@ -4794,26 +4814,6 @@
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4831,131 +4831,131 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="29" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="29" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="29" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="29" t="s">
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="29" t="s">
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="31"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="28"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="28"/>
+      <c r="N2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30" t="s">
+      <c r="O2" s="27"/>
+      <c r="P2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30" t="s">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="29" t="s">
+      <c r="S2" s="28"/>
+      <c r="T2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30" t="s">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30" t="s">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="29" t="s">
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="29" t="s">
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30" t="s">
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="31"/>
+      <c r="AK2" s="28"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
@@ -6416,6 +6416,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="Z1:AE1"/>
     <mergeCell ref="AF1:AK1"/>
     <mergeCell ref="L2:M2"/>
@@ -6432,14 +6440,6 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6449,8 +6449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CD2424-D863-F54D-9F28-8797A24212D3}">
   <dimension ref="B3:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>